<commit_message>
Add weights and estimator sections to Chapter 3 Method
</commit_message>
<xml_diff>
--- a/Model building/Cronbach.xlsx
+++ b/Model building/Cronbach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BC25ED-261C-4733-BB14-0A0EC317CEC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6CD588-95F5-403D-B907-59BB0400B5A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12840" windowWidth="18240" windowHeight="28440" xr2:uid="{7461CD50-8584-4B05-B8A2-9D4B61CECD4C}"/>
   </bookViews>
@@ -615,7 +615,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Complete Chapter 3 Method
</commit_message>
<xml_diff>
--- a/Model building/Cronbach.xlsx
+++ b/Model building/Cronbach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6CD588-95F5-403D-B907-59BB0400B5A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE719B-4B5D-4B3E-9651-67CBD5CB3286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12840" windowWidth="18240" windowHeight="28440" xr2:uid="{7461CD50-8584-4B05-B8A2-9D4B61CECD4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7461CD50-8584-4B05-B8A2-9D4B61CECD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Country</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Partner countries</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -189,7 +186,13 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Item parameters</t>
+    <t>Reference for</t>
+  </si>
+  <si>
+    <t>scale reliabilities</t>
+  </si>
+  <si>
+    <t>Reference for item parameters</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -270,9 +273,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,11 +292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,7 +615,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,34 +626,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="D2" s="7"/>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
@@ -672,617 +676,621 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
+      <c r="A3" s="2">
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>76</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="8">
         <v>0.89600000000000002</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0.871</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0.79400000000000004</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>0.85799999999999998</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8">
         <v>0.92900000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
+      <c r="A4" s="2">
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
-        <v>100</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="8">
         <v>0.91200000000000003</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>0.83599999999999997</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.85099999999999998</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>0.81399999999999995</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8">
         <v>0.92700000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
+      <c r="A5" s="2">
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
-        <v>124</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8">
         <v>0.90400000000000003</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>0.85599999999999998</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.75800000000000001</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0.81599999999999995</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8">
         <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
+      <c r="A6" s="2">
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
-        <v>152</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8">
         <v>0.88500000000000001</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>0.85099999999999998</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>0.81799999999999995</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8">
         <v>0.91500000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
+      <c r="A7" s="2">
+        <v>233</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
-        <v>233</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>0.83299999999999996</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>0.70899999999999996</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>0.752</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8">
         <v>0.872</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
+      <c r="A8" s="2">
+        <v>246</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2">
-        <v>246</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>0.81899999999999995</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>0.76</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>0.78300000000000003</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8">
         <v>0.89600000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
+      <c r="A9" s="2">
+        <v>268</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2">
-        <v>268</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="8">
         <v>0.89100000000000001</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.83399999999999996</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>0.84599999999999997</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>0.86199999999999999</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8">
         <v>0.92</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
+      <c r="A10" s="2">
+        <v>360</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2">
-        <v>360</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="8">
         <v>0.878</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.82699999999999996</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0.75600000000000001</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>0.89200000000000002</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8">
         <v>0.93100000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>34</v>
+      <c r="A11" s="2">
+        <v>380</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2">
-        <v>380</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.79800000000000004</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0.79500000000000004</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>0.84</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9">
+      <c r="I11" s="8"/>
+      <c r="J11" s="8">
         <v>0.89800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
+      <c r="A12" s="2">
+        <v>428</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2">
-        <v>428</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8">
         <v>0.84599999999999997</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>0.81299999999999994</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>0.70299999999999996</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>0.78</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8">
         <v>0.89700000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
+      <c r="A13" s="2">
+        <v>440</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2">
-        <v>440</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8">
         <v>0.90900000000000003</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.86899999999999999</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.84599999999999997</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>0.77900000000000003</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8">
         <v>0.92100000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
+      <c r="A14" s="2">
+        <v>528</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2">
-        <v>528</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="8">
         <v>0.84899999999999998</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>0.79200000000000004</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>0.63800000000000001</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>0.79200000000000004</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8">
         <v>0.874</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>38</v>
+      <c r="A15" s="2">
+        <v>604</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2">
-        <v>604</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="8">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>0.81299999999999994</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>0.75800000000000001</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8">
         <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
+      <c r="A16" s="2">
+        <v>616</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2">
-        <v>616</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8">
         <v>0.878</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>0.83</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>0.77100000000000002</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>0.83899999999999997</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8">
         <v>0.91300000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
+      <c r="A17" s="2">
+        <v>620</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2">
-        <v>620</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="8">
         <v>0.89600000000000002</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>0.84399999999999997</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <v>0.77500000000000002</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>0.84899999999999998</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8">
         <v>0.89900000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
+      <c r="A18" s="2">
+        <v>643</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2">
-        <v>643</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="8">
         <v>0.89200000000000002</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>0.85499999999999998</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>0.72599999999999998</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>0.874</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9">
+      <c r="I18" s="8"/>
+      <c r="J18" s="8">
         <v>0.91100000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
+      <c r="A19" s="2">
+        <v>688</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2">
-        <v>688</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="8">
         <v>0.92600000000000005</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>0.85299999999999998</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0.83799999999999997</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>0.78600000000000003</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8">
         <v>0.93899999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
+      <c r="A20" s="2">
+        <v>703</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2">
-        <v>703</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="8">
         <v>0.874</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>0.82899999999999996</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>0.78300000000000003</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9">
+      <c r="I20" s="8"/>
+      <c r="J20" s="8">
         <v>0.90700000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
+      <c r="A21" s="2">
+        <v>724</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2">
-        <v>724</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="8">
         <v>0.879</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>0.81200000000000006</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>0.77900000000000003</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>0.85399999999999998</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8">
         <v>0.91200000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>45</v>
+      <c r="A22" s="3">
+        <v>840</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3">
-        <v>840</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10">
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="9">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>0.83899999999999997</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>0.75600000000000001</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="9">
         <v>0.88100000000000001</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10">
+      <c r="I22" s="9"/>
+      <c r="J22" s="9">
         <v>0.90900000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="E23" s="13">
+      <c r="E23" s="11">
         <v>16.89</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="11">
         <v>16.89</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="11">
         <v>16.579999999999998</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <v>16.63</v>
       </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13">
+      <c r="I23" s="11"/>
+      <c r="J23" s="11">
         <v>16.89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="11">
         <v>16.899999999999999</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <v>16.899999999999999</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="11">
         <v>16.59</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <v>16.64</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13">
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
         <v>16.899999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="A26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7">
         <v>16.93</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="7">
         <v>16.940000000000001</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="7">
         <v>16.61</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="7">
         <v>16.66</v>
       </c>
-      <c r="J26" s="1">
+      <c r="I26" s="7"/>
+      <c r="J26" s="7">
         <v>16.91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22 J3:J22">
     <cfRule type="dataBar" priority="1">

</xml_diff>

<commit_message>
Complete thesis defence transcript
</commit_message>
<xml_diff>
--- a/Model building/Cronbach.xlsx
+++ b/Model building/Cronbach.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE719B-4B5D-4B3E-9651-67CBD5CB3286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A12AC68-F00E-4CED-91D0-9CCC1C83C670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7461CD50-8584-4B05-B8A2-9D4B61CECD4C}"/>
+    <workbookView xWindow="28680" yWindow="-12840" windowWidth="18240" windowHeight="28440" xr2:uid="{7461CD50-8584-4B05-B8A2-9D4B61CECD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Country</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Reference for item parameters</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -612,20 +618,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677F55F5-43DF-443C-A30B-0BA3FAD1CAA8}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J22"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="9" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -647,7 +653,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>52</v>
       </c>
@@ -675,7 +681,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>76</v>
       </c>
@@ -702,7 +708,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>100</v>
       </c>
@@ -729,7 +735,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>124</v>
       </c>
@@ -756,7 +762,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>152</v>
       </c>
@@ -783,7 +789,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>233</v>
       </c>
@@ -810,7 +816,7 @@
         <v>0.872</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>246</v>
       </c>
@@ -837,7 +843,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>268</v>
       </c>
@@ -864,7 +870,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>360</v>
       </c>
@@ -891,7 +897,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>380</v>
       </c>
@@ -918,7 +924,7 @@
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>428</v>
       </c>
@@ -945,7 +951,7 @@
         <v>0.89700000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>440</v>
       </c>
@@ -972,7 +978,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>528</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>604</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>616</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>620</v>
       </c>
@@ -1080,7 +1086,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>643</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>688</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>0.93899999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>703</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>724</v>
       </c>
@@ -1188,7 +1194,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>840</v>
       </c>
@@ -1216,7 +1222,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>16.89</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>55</v>
       </c>
@@ -1286,6 +1292,58 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7">
         <v>16.91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="8">
+        <f>MIN(E3:E22)</f>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" ref="F28:J28" si="0">MIN(F3:F22)</f>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="0"/>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="H28" s="8">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8">
+        <f t="shared" si="0"/>
+        <v>0.872</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="8">
+        <f>MAX(E3:E22)</f>
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" ref="F29:J29" si="1">MAX(F3:F22)</f>
+        <v>0.871</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="1"/>
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="H29" s="8">
+        <f t="shared" si="1"/>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8">
+        <f t="shared" si="1"/>
+        <v>0.93899999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>